<commit_message>
fix typos and other gremlins
</commit_message>
<xml_diff>
--- a/documents/ipf-table-1.xlsx
+++ b/documents/ipf-table-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
   <si>
     <t xml:space="preserve">Reference
 Author year 
@@ -81,7 +81,7 @@
   <si>
     <t xml:space="preserve">11.0; 
 2.3, 
-52</t>
+52.4</t>
   </si>
   <si>
     <t xml:space="preserve">2.9; 
@@ -209,6 +209,11 @@
 112.4</t>
   </si>
   <si>
+    <t xml:space="preserve">0.6;
+0.2,
+1.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.8;
 0.5,
 7.0</t>
@@ -282,9 +287,9 @@
 6.8</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7;
-0.3,
-1.3</t>
+    <t xml:space="preserve">1;
+0.4,
+2.3</t>
   </si>
   <si>
     <t xml:space="preserve">1.1;
@@ -301,9 +306,9 @@
 22.1</t>
   </si>
   <si>
-    <t xml:space="preserve">1.8;
-1,
-3.1</t>
+    <t xml:space="preserve">3.3;
+1.2,
+10.1</t>
   </si>
   <si>
     <t xml:space="preserve">Paolocci 2013, soft wood (abstract only)
@@ -473,17 +478,20 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3418367346939"/>
+    <col collapsed="false" hidden="true" max="5" min="3" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4489795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,7 +659,7 @@
         <v>30</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>7</v>
@@ -698,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,8 +757,11 @@
       <c r="H8" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>26</v>
@@ -761,13 +772,16 @@
       <c r="M8" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="O8" s="0" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>13</v>
@@ -776,36 +790,39 @@
         <v>140</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="L9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="M9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>13</v>
@@ -814,13 +831,13 @@
         <v>97</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>9</v>
@@ -828,7 +845,7 @@
     </row>
     <row r="11" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>13</v>
@@ -837,21 +854,21 @@
         <v>100</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>13</v>
@@ -860,36 +877,39 @@
         <v>95</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>6</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>13</v>
@@ -898,27 +918,27 @@
         <v>106</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>78</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>13</v>
@@ -927,19 +947,19 @@
         <v>65</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>9</v>
@@ -948,32 +968,35 @@
         <v>2</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>13</v>
@@ -982,22 +1005,22 @@
         <v>78</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>35</v>
@@ -1009,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>